<commit_message>
Added Service Pricing Column
</commit_message>
<xml_diff>
--- a/data_capture/static/data_capture/r3_example.xlsx
+++ b/data_capture/static/data_capture/r3_example.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\calc\data_capture\static\data_capture\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BE24BC-DA01-4DF1-A7B2-B3C9B70DD590}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="770" yWindow="550" windowWidth="17520" windowHeight="8490" activeTab="1"/>
+    <workbookView xWindow="765" yWindow="555" windowWidth="17520" windowHeight="8490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Labor Category" sheetId="2" r:id="rId1"/>
-    <sheet name="I don't know what to upload." sheetId="3" r:id="rId2"/>
+    <sheet name="Service Pricing" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -95,9 +101,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -206,7 +212,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -218,6 +224,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -266,7 +275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,9 +308,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -334,6 +360,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,34 +552,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="11" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="12.7265625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="5" customWidth="1"/>
     <col min="12" max="12" width="14" style="5" customWidth="1"/>
-    <col min="13" max="13" width="16.54296875" style="5" customWidth="1"/>
-    <col min="14" max="14" width="20.08984375" style="5" customWidth="1"/>
-    <col min="15" max="27" width="9.08984375" style="5" customWidth="1"/>
-    <col min="28" max="16384" width="14.453125" style="5"/>
+    <col min="13" max="13" width="16.5703125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" style="5" customWidth="1"/>
+    <col min="15" max="27" width="9.140625" style="5" customWidth="1"/>
+    <col min="28" max="16384" width="14.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A1" s="10"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -591,7 +634,7 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -635,7 +678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>14</v>
       </c>
@@ -686,33 +729,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="8" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="26" width="9.08984375" style="5" customWidth="1"/>
-    <col min="27" max="16384" width="14.453125" style="5"/>
+    <col min="14" max="26" width="9.140625" style="5" customWidth="1"/>
+    <col min="27" max="16384" width="14.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="100" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -766,7 +809,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -791,7 +834,7 @@
       </c>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>

</xml_diff>